<commit_message>
Kurzschlusskräfte: Reverse- und Vorwärts-Mapping-Implementierung ergänzt, neues JSON-Template hinzugefügt, und `mapping.json`/`mappingreversed.json` eingeführt. Validierungslogik und State-Handhabung erweitert. Dokumentation aktualisiert.
</commit_message>
<xml_diff>
--- a/examples/ABB_Schaltanlagenhandbuch_Beispiel_S161.xlsx
+++ b/examples/ABB_Schaltanlagenhandbuch_Beispiel_S161.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29809"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1d3018db502cb77/Documents/GitHub/Kurzschlussfestigkeit/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4F9F0D-A878-4324-AAFE-A0E6D20A0E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{BF4F9F0D-A878-4324-AAFE-A0E6D20A0E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A026CD12-8B6E-44EA-9757-F7B847D3DEB7}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-45" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Höhenkorrektur" sheetId="1" r:id="rId1"/>
-    <sheet name="Quellen &amp; Versionen" sheetId="2" r:id="rId2"/>
+    <sheet name="Kurzschlussfestigkeit Leitersei" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Eingaben für die Kurzschlussfestigkeit bei Leiterseilen</t>
   </si>
@@ -47,9 +46,6 @@
     <t>Höhenunterschied der Befestigungspunkte mehr als 25%</t>
   </si>
   <si>
-    <t>Schlaufebene bei Schlaufen in Spannfeldmitte</t>
-  </si>
-  <si>
     <t>ϑ_l Niedrigste Temperatur</t>
   </si>
   <si>
@@ -149,37 +145,19 @@
     <t>Abstand Phasenabstandshalter 10</t>
   </si>
   <si>
-    <t>Relevante Dokumente (nicht abschliessend)</t>
-  </si>
-  <si>
-    <t>Versionskontrolle</t>
-  </si>
-  <si>
-    <t>Dokument</t>
-  </si>
-  <si>
-    <t>Änderungsgrund</t>
-  </si>
-  <si>
-    <t>Revision</t>
-  </si>
-  <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>[1] Starkstromverordnung Anhang 2</t>
-  </si>
-  <si>
-    <t>Initiale Erstellung</t>
-  </si>
-  <si>
-    <t>AnRu</t>
-  </si>
-  <si>
-    <t>[2] IEC 60071-2, Kapitel 4.2.2</t>
+    <t>Schlaufengeometrie bei Schlaufen in Spannfeldmitte</t>
+  </si>
+  <si>
+    <t>h Schlaufenhöhe</t>
+  </si>
+  <si>
+    <t>w Schlaufenbreite</t>
+  </si>
+  <si>
+    <t>l_v Seilbogenlänge der Schlaufe</t>
+  </si>
+  <si>
+    <t>Schlaufenebene bei Schlaufen in Spannfeldmitte</t>
   </si>
 </sst>
 </file>
@@ -197,7 +175,7 @@
     <numFmt numFmtId="171" formatCode="#,##0\ &quot;N/m&quot;"/>
     <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;Hz&quot;"/>
     <numFmt numFmtId="173" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -361,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -443,7 +421,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -459,6 +437,47 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -472,6 +491,34 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -482,23 +529,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -511,112 +545,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -641,7 +569,7 @@
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="174" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2"/>
@@ -654,7 +582,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -666,11 +594,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -679,135 +607,71 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="11" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="172" fontId="11" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21" hidden="1"/>
@@ -836,6 +700,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1043,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:B30"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1074,19 +942,19 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1095,7 +963,7 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
@@ -1107,7 +975,7 @@
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1"/>
@@ -1119,7 +987,7 @@
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
@@ -1129,9 +997,9 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="37"/>
+        <v>45</v>
+      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1139,249 +1007,261 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="29">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13">
         <v>-20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="30">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="43"/>
+      <c r="B11" s="32"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="31">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="39">
+        <v>12</v>
+      </c>
+      <c r="B13" s="23">
         <v>1.7669999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="32">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="38">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="43"/>
+      <c r="B16" s="32"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="28">
+        <v>18</v>
+      </c>
+      <c r="B18" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="17">
+        <v>93.015000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="33">
-        <v>93.015000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="43"/>
+      <c r="B20" s="32"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="25">
+        <v>21</v>
+      </c>
+      <c r="B21" s="10">
         <v>42.5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="25">
+        <v>22</v>
+      </c>
+      <c r="B22" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="25"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="25">
+        <v>24</v>
+      </c>
+      <c r="B24" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="25">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="43"/>
+      <c r="B26" s="32"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="34">
+        <v>27</v>
+      </c>
+      <c r="B27" s="18">
         <v>12.1264</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="34">
+        <v>28</v>
+      </c>
+      <c r="B28" s="18">
         <v>11.3704</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="19">
+        <v>480500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="35">
-        <v>480500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="43"/>
+      <c r="B30" s="32"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="25">
+        <v>31</v>
+      </c>
+      <c r="B31" s="10">
         <v>6.5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="25">
+        <v>32</v>
+      </c>
+      <c r="B32" s="10">
         <v>6.5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="25">
+        <v>33</v>
+      </c>
+      <c r="B33" s="10">
         <v>6.5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="25">
+        <v>34</v>
+      </c>
+      <c r="B34" s="10">
         <v>6.5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="25">
+        <v>35</v>
+      </c>
+      <c r="B35" s="10">
         <v>6.5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="25"/>
+        <v>36</v>
+      </c>
+      <c r="B36" s="10"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="25"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="25"/>
+        <v>38</v>
+      </c>
+      <c r="B38" s="10"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="10"/>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="25"/>
-    </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
+      <c r="B40" s="10"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="27"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="B41" s="26"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="10"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A43" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="10"/>
+    </row>
+    <row r="44" spans="1:2" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
@@ -1515,7 +1395,11 @@
       <c r="E73" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <protectedRanges>
+    <protectedRange sqref="B41:B44" name="Bereich2"/>
+  </protectedRanges>
+  <mergeCells count="8">
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A20:B20"/>
@@ -1524,7 +1408,7 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A11:B11"/>
   </mergeCells>
-  <dataValidations count="10">
+  <dataValidations disablePrompts="1" count="10">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Abgespannt, Aufgelegt, Unterschlaufung, Schlaufe am Spannfeldende"</formula1>
     </dataValidation>
@@ -1560,298 +1444,10 @@
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"-,Fett"&amp;8</oddHeader>
-    <oddFooter>&amp;L&amp;8 Kurzschlussfestigkeit bei Leiterseilen
+    <oddFooter>&amp;L&amp;"Aptos,Standard"&amp;8Kurzschlussfestigkeit bei Leiterseilen
 Rev. 0.0&amp;C&amp;"Aptos,Standard" Stationsname
-Projektbeschreibung&amp;R&amp;8 &amp;P/&amp;N</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F27"/>
-  <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="64.625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="37.875" style="4" customWidth="1"/>
-    <col min="4" max="6" width="13.375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.75" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.75" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="13">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
-        <v>45916</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="24"/>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L3JGn++vkSXlWLsCCYWWINtqUqmHh3ss+Y3UnfzvYnEO110ZTLt4h5Wk1J0P8sdh9gATNb+6gDKHOpRAIsir+Q==" saltValue="aQCLb7ecvUo3cSUIR9a0KA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="25">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A9:B9"/>
-  </mergeCells>
-  <pageMargins left="0.78740157480314965" right="0.55118110236220474" top="1.181102362204725" bottom="0.9055118110236221" header="0.47244094488188981" footer="0.35433070866141742"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0">
-    <oddHeader>&amp;L&amp;G&amp;C&amp;"-,Fett"&amp;8</oddHeader>
-    <oddFooter>&amp;L&amp;8 Berechnung von Erdergeometrien
-Rev. 0.0&amp;C&amp;"Aptos,Standard" Stationsname
-Projektbeschreibung&amp;R&amp;8 &amp;P/&amp;N</oddFooter>
+Projektbeschreibung
+&amp;F&amp;R&amp;"Aptos,Standard"&amp;8 &amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>